<commit_message>
UR 1.9 blank upload
</commit_message>
<xml_diff>
--- a/Emergency Department/capacity redesign.xlsx
+++ b/Emergency Department/capacity redesign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\irnhsft.local\monitor\Redirected\paul.bullard\Documents\GitHub\EDDemandandCapacity1\Emergency Department\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78A581FA-B947-455E-AF57-15C3386C376D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0DDD97C-BF7D-4996-A449-11B4FF0C6736}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="1425" windowWidth="29040" windowHeight="15840" xr2:uid="{21D17A18-EA42-406F-93DA-4215455D9962}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Dr Smith</t>
+  </si>
+  <si>
+    <t>Dr Nights Pattern 1</t>
   </si>
 </sst>
 </file>
@@ -131,8 +134,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -157,7 +161,7 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>66675</xdr:colOff>
+          <xdr:colOff>69850</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
@@ -165,7 +169,7 @@
           <xdr:col>11</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>23</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>146050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -175,7 +179,7 @@
                   <a14:compatExt spid="_x0000_s4097"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC6220A9-7A42-44E0-A2D8-06763B117C52}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -196,23 +200,10 @@
               <a:solidFill>
                 <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
+              <a:tailEnd/>
             </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -523,7 +514,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -566,7 +557,7 @@
   <dimension ref="B2:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -614,6 +605,12 @@
       <c r="B3" t="s">
         <v>13</v>
       </c>
+      <c r="C3" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.70833333333333337</v>
+      </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
@@ -640,10 +637,13 @@
   <dimension ref="B1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
@@ -678,7 +678,7 @@
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -714,7 +714,7 @@
   <dimension ref="B1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>